<commit_message>
Fixed spaces on end of names
</commit_message>
<xml_diff>
--- a/BROMappings/Mapping en definitie BRO GMW.xlsx
+++ b/BROMappings/Mapping en definitie BRO GMW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/Datamodels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\RWS Ketentest\pybron\BronDatamodel\BROMappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{C98B97DB-AF31-43E8-BA33-4B0785DBF11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30B8BD1A-CF02-4848-93DD-BACA524CE8A3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB233E5-5F60-4464-8750-9C3F62CEA0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="322">
   <si>
     <t xml:space="preserve">RegistrationObject </t>
   </si>
@@ -711,9 +711,6 @@
     <t>referentiestelsel</t>
   </si>
   <si>
-    <t xml:space="preserve">methode locatiebepaling </t>
-  </si>
-  <si>
     <t>lokaal verticaal referentiepunt</t>
   </si>
   <si>
@@ -777,12 +774,6 @@
     <t>elektrodepositie</t>
   </si>
   <si>
-    <t xml:space="preserve">elektrodestatus </t>
-  </si>
-  <si>
-    <t xml:space="preserve">aanvulmateriaal buis </t>
-  </si>
-  <si>
     <t>lijm</t>
   </si>
   <si>
@@ -792,9 +783,6 @@
     <t>filterlengte</t>
   </si>
   <si>
-    <t xml:space="preserve">kousmateriaal </t>
-  </si>
-  <si>
     <t>zandvanglengte</t>
   </si>
   <si>
@@ -991,6 +979,21 @@
   </si>
   <si>
     <t>(Nu nog) Index van C.DATA.BRO.COM.List.QualityRegime</t>
+  </si>
+  <si>
+    <t>methode locatiebepaling</t>
+  </si>
+  <si>
+    <t>aanvulmateriaal buis</t>
+  </si>
+  <si>
+    <t>kousmateriaal</t>
+  </si>
+  <si>
+    <t>elektrodestatus</t>
+  </si>
+  <si>
+    <t>sedSumpLength</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1158,30 +1161,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1450,35 +1429,35 @@
   <dimension ref="A1:T91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2784" ySplit="696" topLeftCell="Q1" activePane="bottomRight"/>
+      <pane xSplit="2790" ySplit="690" topLeftCell="J57" activePane="bottomRight"/>
       <selection activeCell="D5" sqref="D5"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
-      <selection pane="bottomRight" activeCell="T21" sqref="T21"/>
+      <selection pane="bottomRight" activeCell="P75" sqref="P75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.44140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="25.33203125" customWidth="1"/>
-    <col min="18" max="18" width="26.33203125" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="77.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="25.28515625" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="77.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>191</v>
       </c>
@@ -1540,7 +1519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1570,7 +1549,7 @@
         <v>89</v>
       </c>
       <c r="O2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P2" t="s">
         <v>185</v>
@@ -1585,7 +1564,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1630,7 +1609,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1675,7 +1654,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1689,7 +1668,7 @@
         <v>42</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>89</v>
@@ -1714,16 +1693,16 @@
         <v>169</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>84</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1738,10 +1717,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H6" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="J6" s="6">
         <v>1</v>
@@ -1753,7 +1732,7 @@
         <v>84</v>
       </c>
       <c r="O6" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P6" t="s">
         <v>101</v>
@@ -1768,7 +1747,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1786,7 +1765,7 @@
         <v>207</v>
       </c>
       <c r="H7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="J7" s="6">
         <v>1</v>
@@ -1798,10 +1777,10 @@
         <v>84</v>
       </c>
       <c r="N7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="O7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P7" t="s">
         <v>103</v>
@@ -1819,7 +1798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1837,7 +1816,7 @@
         <v>208</v>
       </c>
       <c r="H8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="J8" s="6">
         <v>1</v>
@@ -1849,7 +1828,7 @@
         <v>84</v>
       </c>
       <c r="N8" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="O8" t="s">
         <v>102</v>
@@ -1867,7 +1846,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1885,7 +1864,7 @@
         <v>209</v>
       </c>
       <c r="H9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="J9" s="6">
         <v>1</v>
@@ -1897,16 +1876,16 @@
         <v>84</v>
       </c>
       <c r="N9" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="O9" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P9" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Q9" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="R9" s="6" t="s">
         <v>111</v>
@@ -1918,7 +1897,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1935,7 +1914,7 @@
         <v>210</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J10" s="16">
         <v>1</v>
@@ -1947,10 +1926,10 @@
         <v>84</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="O10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>184</v>
@@ -1965,49 +1944,49 @@
         <v>84</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
+        <v>256</v>
+      </c>
+      <c r="D11" t="s">
+        <v>257</v>
+      </c>
+      <c r="E11" t="s">
+        <v>258</v>
+      </c>
+      <c r="F11" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" t="s">
         <v>260</v>
       </c>
-      <c r="D11" t="s">
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>84</v>
+      </c>
+      <c r="N11" t="s">
         <v>261</v>
       </c>
-      <c r="E11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F11" t="s">
-        <v>263</v>
-      </c>
-      <c r="H11" t="s">
-        <v>264</v>
-      </c>
-      <c r="J11" s="6">
-        <v>1</v>
-      </c>
-      <c r="K11" s="6">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
-        <v>84</v>
-      </c>
-      <c r="N11" t="s">
-        <v>265</v>
-      </c>
       <c r="O11" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P11" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="Q11" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="R11" t="s">
         <v>168</v>
@@ -2016,7 +1995,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2056,13 +2035,13 @@
       </c>
       <c r="N12"/>
       <c r="O12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P12" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="Q12" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>107</v>
@@ -2071,28 +2050,28 @@
         <v>84</v>
       </c>
       <c r="T12" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D13" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E13" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F13" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H13" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J13" s="6">
         <v>1</v>
@@ -2104,7 +2083,7 @@
         <v>84</v>
       </c>
       <c r="N13" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="O13" t="s">
         <v>146</v>
@@ -2122,25 +2101,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
+        <v>256</v>
+      </c>
+      <c r="D14" t="s">
+        <v>257</v>
+      </c>
+      <c r="E14" t="s">
+        <v>266</v>
+      </c>
+      <c r="F14" t="s">
+        <v>267</v>
+      </c>
+      <c r="H14" t="s">
         <v>260</v>
-      </c>
-      <c r="D14" t="s">
-        <v>261</v>
-      </c>
-      <c r="E14" t="s">
-        <v>270</v>
-      </c>
-      <c r="F14" t="s">
-        <v>271</v>
-      </c>
-      <c r="H14" t="s">
-        <v>264</v>
       </c>
       <c r="J14" s="6">
         <v>0</v>
@@ -2152,7 +2131,7 @@
         <v>84</v>
       </c>
       <c r="N14" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="O14" t="s">
         <v>146</v>
@@ -2170,28 +2149,28 @@
         <v>83</v>
       </c>
       <c r="T14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15"/>
       <c r="C15" t="s">
+        <v>256</v>
+      </c>
+      <c r="D15" t="s">
+        <v>257</v>
+      </c>
+      <c r="E15" t="s">
+        <v>269</v>
+      </c>
+      <c r="F15" t="s">
+        <v>270</v>
+      </c>
+      <c r="H15" t="s">
         <v>260</v>
-      </c>
-      <c r="D15" t="s">
-        <v>261</v>
-      </c>
-      <c r="E15" t="s">
-        <v>273</v>
-      </c>
-      <c r="F15" t="s">
-        <v>274</v>
-      </c>
-      <c r="H15" t="s">
-        <v>264</v>
       </c>
       <c r="J15" s="6">
         <v>0</v>
@@ -2203,7 +2182,7 @@
         <v>84</v>
       </c>
       <c r="N15" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="O15" t="s">
         <v>146</v>
@@ -2221,25 +2200,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E16" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F16" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H16" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J16" s="6">
         <v>1</v>
@@ -2251,7 +2230,7 @@
         <v>84</v>
       </c>
       <c r="N16" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="O16" t="s">
         <v>146</v>
@@ -2269,25 +2248,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17"/>
       <c r="C17" t="s">
+        <v>256</v>
+      </c>
+      <c r="D17" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17" t="s">
+        <v>275</v>
+      </c>
+      <c r="F17" t="s">
+        <v>276</v>
+      </c>
+      <c r="H17" t="s">
         <v>260</v>
-      </c>
-      <c r="D17" t="s">
-        <v>261</v>
-      </c>
-      <c r="E17" t="s">
-        <v>279</v>
-      </c>
-      <c r="F17" t="s">
-        <v>280</v>
-      </c>
-      <c r="H17" t="s">
-        <v>264</v>
       </c>
       <c r="J17" s="6">
         <v>0</v>
@@ -2299,7 +2278,7 @@
         <v>84</v>
       </c>
       <c r="N17" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="O17" t="s">
         <v>146</v>
@@ -2317,25 +2296,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
       <c r="B18"/>
       <c r="C18" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D18" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E18" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F18" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H18" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J18" s="6">
         <v>1</v>
@@ -2347,7 +2326,7 @@
         <v>84</v>
       </c>
       <c r="N18" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="O18" t="s">
         <v>9</v>
@@ -2365,25 +2344,25 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19"/>
       <c r="C19" t="s">
+        <v>256</v>
+      </c>
+      <c r="D19" t="s">
+        <v>257</v>
+      </c>
+      <c r="E19" t="s">
+        <v>281</v>
+      </c>
+      <c r="F19" t="s">
+        <v>282</v>
+      </c>
+      <c r="H19" t="s">
         <v>260</v>
-      </c>
-      <c r="D19" t="s">
-        <v>261</v>
-      </c>
-      <c r="E19" t="s">
-        <v>285</v>
-      </c>
-      <c r="F19" t="s">
-        <v>286</v>
-      </c>
-      <c r="H19" t="s">
-        <v>264</v>
       </c>
       <c r="J19" s="6">
         <v>0</v>
@@ -2395,7 +2374,7 @@
         <v>84</v>
       </c>
       <c r="N19" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="O19" t="s">
         <v>9</v>
@@ -2413,25 +2392,25 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D20" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E20" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F20" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H20" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J20" s="6">
         <v>1</v>
@@ -2443,7 +2422,7 @@
         <v>84</v>
       </c>
       <c r="N20" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="O20" t="s">
         <v>9</v>
@@ -2461,25 +2440,25 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="B21"/>
       <c r="C21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" t="s">
+        <v>257</v>
+      </c>
+      <c r="E21" t="s">
+        <v>287</v>
+      </c>
+      <c r="F21" t="s">
+        <v>288</v>
+      </c>
+      <c r="H21" t="s">
         <v>260</v>
-      </c>
-      <c r="D21" t="s">
-        <v>261</v>
-      </c>
-      <c r="E21" t="s">
-        <v>291</v>
-      </c>
-      <c r="F21" t="s">
-        <v>292</v>
-      </c>
-      <c r="H21" t="s">
-        <v>264</v>
       </c>
       <c r="J21" s="6">
         <v>0</v>
@@ -2491,7 +2470,7 @@
         <v>84</v>
       </c>
       <c r="N21" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="O21" t="s">
         <v>9</v>
@@ -2509,25 +2488,25 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D22" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E22" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F22" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="H22" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J22" s="6">
         <v>1</v>
@@ -2539,7 +2518,7 @@
         <v>84</v>
       </c>
       <c r="N22" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="O22" t="s">
         <v>9</v>
@@ -2557,24 +2536,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="J23" s="16">
         <v>0</v>
@@ -2586,7 +2565,7 @@
         <v>84</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>9</v>
@@ -2604,7 +2583,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2649,7 +2628,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2694,7 +2673,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2739,7 +2718,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2784,7 +2763,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2832,7 +2811,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -2880,7 +2859,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2928,7 +2907,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2961,10 +2940,10 @@
         <v>102</v>
       </c>
       <c r="P31" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="Q31" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="R31" s="1" t="s">
         <v>106</v>
@@ -2974,7 +2953,7 @@
       </c>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -3019,7 +2998,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -3049,7 +3028,7 @@
         <v>84</v>
       </c>
       <c r="O33" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P33" t="s">
         <v>118</v>
@@ -3067,7 +3046,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -3115,7 +3094,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -3166,7 +3145,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>13</v>
       </c>
@@ -3214,7 +3193,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -3262,7 +3241,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -3310,13 +3289,13 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
       <c r="B39"/>
       <c r="C39" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -3355,13 +3334,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
       <c r="B40"/>
       <c r="C40" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
@@ -3403,7 +3382,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -3448,7 +3427,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -3493,7 +3472,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -3508,7 +3487,7 @@
         <v>32</v>
       </c>
       <c r="F43" t="s">
-        <v>227</v>
+        <v>317</v>
       </c>
       <c r="J43" s="6">
         <v>1</v>
@@ -3535,7 +3514,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -3550,7 +3529,7 @@
         <v>35</v>
       </c>
       <c r="F44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J44" s="6">
         <v>1</v>
@@ -3580,7 +3559,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -3595,7 +3574,7 @@
         <v>36</v>
       </c>
       <c r="F45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J45" s="6">
         <v>1</v>
@@ -3625,7 +3604,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -3640,7 +3619,7 @@
         <v>37</v>
       </c>
       <c r="F46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J46" s="6">
         <v>1</v>
@@ -3670,7 +3649,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -3685,7 +3664,7 @@
         <v>38</v>
       </c>
       <c r="F47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J47" s="6">
         <v>1</v>
@@ -3715,7 +3694,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>13</v>
       </c>
@@ -3729,7 +3708,7 @@
         <v>39</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J48" s="16">
         <v>1</v>
@@ -3760,7 +3739,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -3775,7 +3754,7 @@
         <v>42</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -3799,13 +3778,13 @@
         <v>169</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="S49" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -3820,7 +3799,7 @@
         <v>43</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -3850,7 +3829,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -3865,7 +3844,7 @@
         <v>44</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -3895,7 +3874,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -3910,7 +3889,7 @@
         <v>45</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -3943,7 +3922,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -3958,7 +3937,7 @@
         <v>46</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -3991,7 +3970,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -4039,7 +4018,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -4054,7 +4033,7 @@
         <v>47</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -4087,7 +4066,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -4102,7 +4081,7 @@
         <v>48</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -4135,7 +4114,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -4150,7 +4129,7 @@
         <v>49</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -4186,7 +4165,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -4201,7 +4180,7 @@
         <v>51</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -4234,7 +4213,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -4249,7 +4228,7 @@
         <v>52</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -4282,7 +4261,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>13</v>
       </c>
@@ -4296,7 +4275,7 @@
         <v>96</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -4330,7 +4309,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -4345,7 +4324,7 @@
         <v>55</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -4378,7 +4357,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -4393,7 +4372,7 @@
         <v>97</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -4423,7 +4402,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -4438,7 +4417,7 @@
         <v>58</v>
       </c>
       <c r="F63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J63" s="6">
         <v>1</v>
@@ -4468,7 +4447,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -4483,7 +4462,7 @@
         <v>59</v>
       </c>
       <c r="F64" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J64" s="6">
         <v>1</v>
@@ -4513,7 +4492,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -4528,7 +4507,7 @@
         <v>60</v>
       </c>
       <c r="F65" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J65" s="6">
         <v>1</v>
@@ -4561,7 +4540,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>13</v>
       </c>
@@ -4575,7 +4554,7 @@
         <v>61</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>249</v>
+        <v>320</v>
       </c>
       <c r="J66" s="16">
         <v>1</v>
@@ -4609,7 +4588,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -4624,7 +4603,7 @@
         <v>64</v>
       </c>
       <c r="F67" t="s">
-        <v>250</v>
+        <v>318</v>
       </c>
       <c r="J67" s="6">
         <v>1</v>
@@ -4651,7 +4630,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -4666,7 +4645,7 @@
         <v>65</v>
       </c>
       <c r="F68" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J68" s="6">
         <v>1</v>
@@ -4696,7 +4675,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -4711,7 +4690,7 @@
         <v>66</v>
       </c>
       <c r="F69" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J69" s="6">
         <v>1</v>
@@ -4741,7 +4720,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -4756,7 +4735,7 @@
         <v>69</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -4789,7 +4768,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -4804,7 +4783,7 @@
         <v>70</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>254</v>
+        <v>319</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -4834,7 +4813,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -4876,7 +4855,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -4918,7 +4897,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -4966,7 +4945,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -4981,7 +4960,7 @@
         <v>77</v>
       </c>
       <c r="F75" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J75" s="6">
         <v>0</v>
@@ -4996,7 +4975,7 @@
         <v>128</v>
       </c>
       <c r="P75" t="s">
-        <v>144</v>
+        <v>321</v>
       </c>
       <c r="Q75" t="s">
         <v>144</v>
@@ -5008,7 +4987,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -5023,7 +5002,7 @@
         <v>80</v>
       </c>
       <c r="F76" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="J76" s="6">
         <v>0</v>
@@ -5053,7 +5032,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -5068,7 +5047,7 @@
         <v>81</v>
       </c>
       <c r="F77" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="J77" s="6">
         <v>0</v>
@@ -5098,7 +5077,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:20" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>13</v>
       </c>
@@ -5112,7 +5091,7 @@
         <v>82</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="J78" s="20">
         <v>0</v>
@@ -5143,7 +5122,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -5197,7 +5176,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -5251,7 +5230,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -5305,7 +5284,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>9</v>
       </c>
@@ -5359,7 +5338,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -5413,7 +5392,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -5467,7 +5446,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -5521,7 +5500,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -5563,10 +5542,10 @@
         <v>128</v>
       </c>
       <c r="P86" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="Q86" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="R86" t="s">
         <v>112</v>
@@ -5575,7 +5554,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -5590,7 +5569,7 @@
         <v>164</v>
       </c>
       <c r="F87" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G87" s="6" t="s">
         <v>89</v>
@@ -5629,7 +5608,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -5644,7 +5623,7 @@
         <v>165</v>
       </c>
       <c r="F88" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>89</v>
@@ -5683,7 +5662,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>9</v>
       </c>
@@ -5737,7 +5716,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -5791,7 +5770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Minor update (datatype and attributename)
tubeInUse, cableInUse, sedimentSumpPresent now have '[NaNBoolean]', as datatype, FilterLevel is now named screenPosition
</commit_message>
<xml_diff>
--- a/BROMappings/Mapping en definitie BRO GMW.xlsx
+++ b/BROMappings/Mapping en definitie BRO GMW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/BronDatamodel/BROMappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{C98B97DB-AF31-43E8-BA33-4B0785DBF11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D286E043-21FA-4858-9C18-BE7C90252065}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{C98B97DB-AF31-43E8-BA33-4B0785DBF11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47BE3D7E-FE4E-467A-BEC4-DB1733279646}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="326">
   <si>
     <t>Registratieobject</t>
   </si>
@@ -1000,6 +1000,12 @@
   </si>
   <si>
     <t>Index van C.DATA.BRO.COM.List.QualityRegime</t>
+  </si>
+  <si>
+    <t>screenTopPosition</t>
+  </si>
+  <si>
+    <t>screenBottomPosition</t>
   </si>
 </sst>
 </file>
@@ -1458,36 +1464,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O44" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2865" ySplit="705" topLeftCell="I1" activePane="bottomRight"/>
+    <sheetView tabSelected="1" topLeftCell="O51" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2892" ySplit="732" topLeftCell="A55" activePane="bottomRight"/>
       <selection activeCell="D5" sqref="D5"/>
       <selection pane="topRight" activeCell="F44" sqref="F1:F1048576"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="A4:XFD4"/>
-      <selection pane="bottomRight" activeCell="T16" sqref="T16"/>
+      <selection pane="bottomRight" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.44140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="25.33203125" customWidth="1"/>
-    <col min="18" max="18" width="26.33203125" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="77.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="25.28515625" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="77.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>147</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1597,7 +1603,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1693,7 +1699,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1741,7 +1747,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1837,7 +1843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1885,7 +1891,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1936,7 +1942,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1986,7 +1992,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -2191,7 +2197,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2239,7 +2245,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2287,7 +2293,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2431,7 +2437,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2482,7 +2488,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2530,7 +2536,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2578,7 +2584,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2670,7 +2676,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2718,7 +2724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -2763,7 +2769,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2811,7 +2817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2907,7 +2913,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2952,7 +2958,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2997,7 +3003,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -3045,7 +3051,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -3093,7 +3099,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -3141,7 +3147,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -3187,7 +3193,7 @@
       </c>
       <c r="T35" s="8"/>
     </row>
-    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
@@ -3235,7 +3241,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -3283,7 +3289,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -3424,7 +3430,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -3469,7 +3475,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -3514,7 +3520,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -3556,7 +3562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -3601,7 +3607,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -3646,7 +3652,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -3691,7 +3697,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -3736,7 +3742,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>8</v>
       </c>
@@ -3781,7 +3787,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -3826,7 +3832,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -3916,7 +3922,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -3955,7 +3961,7 @@
         <v>103</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="S52" t="s">
         <v>41</v>
@@ -3964,7 +3970,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -4012,7 +4018,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -4060,7 +4066,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -4108,7 +4114,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -4156,7 +4162,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -4207,7 +4213,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -4255,7 +4261,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -4303,7 +4309,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>8</v>
       </c>
@@ -4341,8 +4347,8 @@
       <c r="Q60" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R60" s="3" t="s">
-        <v>66</v>
+      <c r="R60" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="S60" s="2" t="s">
         <v>41</v>
@@ -4351,7 +4357,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -4399,7 +4405,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -4438,13 +4444,13 @@
         <v>4</v>
       </c>
       <c r="R62" s="1" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="S62" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -4489,7 +4495,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -4582,7 +4588,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>8</v>
       </c>
@@ -4630,7 +4636,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -4672,7 +4678,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -4717,7 +4723,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -4762,7 +4768,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -4810,7 +4816,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -4855,7 +4861,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -4867,7 +4873,7 @@
         <v>35</v>
       </c>
       <c r="E72" t="s">
-        <v>98</v>
+        <v>324</v>
       </c>
       <c r="F72" t="s">
         <v>57</v>
@@ -4897,7 +4903,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -4909,7 +4915,7 @@
         <v>35</v>
       </c>
       <c r="E73" t="s">
-        <v>99</v>
+        <v>325</v>
       </c>
       <c r="F73" t="s">
         <v>58</v>
@@ -4939,7 +4945,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -4987,7 +4993,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -5029,7 +5035,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -5074,7 +5080,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -5119,7 +5125,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="78" spans="1:20" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>8</v>
       </c>
@@ -5164,7 +5170,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>4</v>
       </c>
@@ -5218,7 +5224,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>4</v>
       </c>
@@ -5272,7 +5278,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>4</v>
       </c>
@@ -5326,7 +5332,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -5380,7 +5386,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>4</v>
       </c>
@@ -5434,7 +5440,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -5488,7 +5494,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -5542,7 +5548,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>4</v>
       </c>
@@ -5596,7 +5602,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -5650,7 +5656,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -5704,7 +5710,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -5758,7 +5764,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -5812,7 +5818,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>4</v>
       </c>

</xml_diff>